<commit_message>
Separate projects for server and client
</commit_message>
<xml_diff>
--- a/CW Checklist.xlsx
+++ b/CW Checklist.xlsx
@@ -87,9 +87,6 @@
     <t>Coursework B</t>
   </si>
   <si>
-    <t>The server will autonomously generate a Navigation Mesh appropriate to the created maze.</t>
-  </si>
-  <si>
     <t>The server will inform the client of the maze structure.</t>
   </si>
   <si>
@@ -229,12 +226,28 @@
   <si>
     <t>Change ESC to X</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The server will autonomously generate a Navigation Mesh appropriate to the created maze. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Not needed?)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +272,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -613,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +687,7 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -681,7 +702,7 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +745,7 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -733,7 +754,7 @@
       </c>
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -754,83 +775,83 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="7"/>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="7"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="7"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="7"/>
     </row>
@@ -839,82 +860,82 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="7"/>
     </row>
@@ -923,52 +944,52 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" s="7"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="7"/>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="7"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64" s="7"/>
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B65" s="7"/>
     </row>

</xml_diff>